<commit_message>
Page 1 + Responsive design Done !
</commit_message>
<xml_diff>
--- a/Compte Rendu/Modèle-audit-SEO  -  10 Recomandations.xlsx
+++ b/Compte Rendu/Modèle-audit-SEO  -  10 Recomandations.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="95">
   <si>
     <t>Catégorie</t>
   </si>
@@ -84,15 +84,9 @@
     <t>Attributs incorrectes dans les formulaires page 2</t>
   </si>
   <si>
-    <t>Contraste couleur texte/arrière-plan trop faible</t>
-  </si>
-  <si>
     <t>SEO et Accessibilité</t>
   </si>
   <si>
-    <t>Pas de focus pour les formulaires</t>
-  </si>
-  <si>
     <t>Manque d'attribut "async" ou "defer" pour le chargement des fichiers javascript page 1 et 2</t>
   </si>
   <si>
@@ -135,15 +129,6 @@
     <t>Code superficiel, balises "&lt;div&gt;" et déclarations CSS inutiles, code lourd et trop chargé</t>
   </si>
   <si>
-    <t>Couleur du texte trop proche de celle de l'arrière-plan</t>
-  </si>
-  <si>
-    <t>Utiliser une couleur de texte bien visible comparé à son arrière-plan</t>
-  </si>
-  <si>
-    <t>Utiliser le paramétrage du focus lors de l'utilisation de formulaire sur une page</t>
-  </si>
-  <si>
     <t>Du code CSS est retrouvé dans le code html, pauvre maintenabilité dans le temps</t>
   </si>
   <si>
@@ -210,9 +195,6 @@
     <t>https://openclassrooms.com/fr/</t>
   </si>
   <si>
-    <t>https://www.matthieu-tranvan.fr/</t>
-  </si>
-  <si>
     <t>https://www.giftofspeed.com/</t>
   </si>
   <si>
@@ -315,7 +297,16 @@
     <t>SEO et Preformances</t>
   </si>
   <si>
-    <t>Difficile de se repérer dans les champs de formulaires, pas de changement de couleurs</t>
+    <t>responsive design mal adapté</t>
+  </si>
+  <si>
+    <t>Mauvais affichage du site lors de la réduction de taille de la fenêtre</t>
+  </si>
+  <si>
+    <t>Toujours s'assurer du bon redimensionnement du contenu et du respect de l'affichage selon la taille d'appareil</t>
+  </si>
+  <si>
+    <t>navigateur</t>
   </si>
 </sst>
 </file>
@@ -691,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -745,22 +736,22 @@
     </row>
     <row r="2" spans="1:26" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E2" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -768,10 +759,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>8</v>
@@ -780,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -788,19 +779,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E4" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -811,7 +802,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>13</v>
@@ -820,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -831,16 +822,16 @@
         <v>14</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -848,19 +839,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -871,16 +862,16 @@
         <v>15</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -891,16 +882,16 @@
         <v>16</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E9" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -911,16 +902,16 @@
         <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -931,16 +922,16 @@
         <v>19</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E11" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -948,19 +939,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E12" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -968,19 +959,19 @@
         <v>6</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E13" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -988,19 +979,19 @@
         <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E14" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -1008,19 +999,19 @@
         <v>7</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E15" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -1028,39 +1019,39 @@
         <v>7</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E16" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E17" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1071,19 +1062,19 @@
         <v>7</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="E21" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -1091,19 +1082,19 @@
         <v>7</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="E22" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -1114,21 +1105,21 @@
         <v>17</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E23" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>11</v>
@@ -1143,7 +1134,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -1151,19 +1142,19 @@
         <v>6</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E25" s="9" t="b">
         <v>1</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -1171,19 +1162,19 @@
         <v>6</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E26" s="9" t="b">
         <v>1</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -1191,79 +1182,79 @@
         <v>6</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E27" s="9" t="b">
         <v>1</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E28" s="14" t="b">
         <v>1</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E29" s="14" t="b">
         <v>1</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E30" s="14" t="b">
         <v>1</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2248,8 +2239,8 @@
     <hyperlink ref="F25" r:id="rId10"/>
     <hyperlink ref="F24" r:id="rId11"/>
     <hyperlink ref="F27" r:id="rId12"/>
-    <hyperlink ref="F21" r:id="rId13"/>
-    <hyperlink ref="F7" r:id="rId14"/>
+    <hyperlink ref="F7" r:id="rId13"/>
+    <hyperlink ref="F22" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId15"/>

</xml_diff>